<commit_message>
File import uses orval.
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eren\Desktop\codes\Python\Django\ses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{289AFE01-B06D-4B4B-843F-56E50E81E702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC8B313B-67D4-4A9D-A881-701AEE76779D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="915" yWindow="360" windowWidth="15990" windowHeight="15240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Page 1" sheetId="1" r:id="rId1"/>
@@ -1936,8 +1936,8 @@
   </sheetPr>
   <dimension ref="A1:K60"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G9" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="J55" sqref="J55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3594,10 +3594,18 @@
       <c r="F50" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G50" s="8"/>
-      <c r="H50" s="8"/>
-      <c r="I50" s="8"/>
-      <c r="J50" s="8"/>
+      <c r="G50" s="8">
+        <v>60</v>
+      </c>
+      <c r="H50" s="8">
+        <v>60</v>
+      </c>
+      <c r="I50" s="8">
+        <v>60</v>
+      </c>
+      <c r="J50" s="8">
+        <v>60</v>
+      </c>
       <c r="K50" s="8"/>
     </row>
     <row r="51" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Implemented course detail to orval.
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eren\Desktop\codes\Python\Django\ses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC8B313B-67D4-4A9D-A881-701AEE76779D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{816FA4A5-3022-4CA5-9E1C-04EEB36958F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Page 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -761,7 +774,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
@@ -787,6 +800,9 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1936,8 +1952,8 @@
   </sheetPr>
   <dimension ref="A1:K60"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="J55" sqref="J55"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:J50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2010,17 +2026,21 @@
       <c r="F2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="6">
-        <v>60</v>
-      </c>
-      <c r="H2" s="6">
-        <v>60</v>
-      </c>
-      <c r="I2" s="6">
-        <v>60</v>
-      </c>
-      <c r="J2" s="6">
-        <v>60</v>
+      <c r="G2" s="9">
+        <f ca="1">TRUNC(RAND()*100)</f>
+        <v>34</v>
+      </c>
+      <c r="H2" s="9">
+        <f t="shared" ref="H2:J17" ca="1" si="0">TRUNC(RAND()*100)</f>
+        <v>96</v>
+      </c>
+      <c r="I2" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="J2" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>38</v>
       </c>
       <c r="K2" s="6"/>
     </row>
@@ -2043,17 +2063,21 @@
       <c r="F3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="6">
-        <v>60</v>
-      </c>
-      <c r="H3" s="6">
-        <v>60</v>
-      </c>
-      <c r="I3" s="6">
-        <v>60</v>
-      </c>
-      <c r="J3" s="6">
-        <v>60</v>
+      <c r="G3" s="9">
+        <f t="shared" ref="G3:J50" ca="1" si="1">TRUNC(RAND()*100)</f>
+        <v>97</v>
+      </c>
+      <c r="H3" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="I3" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="J3" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>58</v>
       </c>
       <c r="K3" s="8"/>
     </row>
@@ -2076,17 +2100,21 @@
       <c r="F4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="6">
-        <v>60</v>
-      </c>
-      <c r="H4" s="6">
-        <v>60</v>
-      </c>
-      <c r="I4" s="6">
-        <v>60</v>
-      </c>
-      <c r="J4" s="6">
-        <v>60</v>
+      <c r="G4" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="H4" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>68</v>
+      </c>
+      <c r="I4" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="J4" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>95</v>
       </c>
       <c r="K4" s="8"/>
     </row>
@@ -2109,17 +2137,21 @@
       <c r="F5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="6">
-        <v>60</v>
-      </c>
-      <c r="H5" s="6">
-        <v>60</v>
-      </c>
-      <c r="I5" s="6">
-        <v>60</v>
-      </c>
-      <c r="J5" s="6">
-        <v>60</v>
+      <c r="G5" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="H5" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="I5" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>68</v>
+      </c>
+      <c r="J5" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>76</v>
       </c>
       <c r="K5" s="8"/>
     </row>
@@ -2142,17 +2174,21 @@
       <c r="F6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="6">
-        <v>60</v>
-      </c>
-      <c r="H6" s="6">
-        <v>60</v>
-      </c>
-      <c r="I6" s="6">
-        <v>60</v>
-      </c>
-      <c r="J6" s="6">
-        <v>60</v>
+      <c r="G6" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>88</v>
+      </c>
+      <c r="H6" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="I6" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>99</v>
+      </c>
+      <c r="J6" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
       </c>
       <c r="K6" s="8"/>
     </row>
@@ -2175,17 +2211,21 @@
       <c r="F7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="6">
-        <v>60</v>
-      </c>
-      <c r="H7" s="6">
-        <v>60</v>
-      </c>
-      <c r="I7" s="6">
-        <v>60</v>
-      </c>
-      <c r="J7" s="6">
-        <v>60</v>
+      <c r="G7" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="H7" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="I7" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>67</v>
+      </c>
+      <c r="J7" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>31</v>
       </c>
       <c r="K7" s="8"/>
     </row>
@@ -2208,17 +2248,21 @@
       <c r="F8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="6">
-        <v>60</v>
-      </c>
-      <c r="H8" s="6">
-        <v>60</v>
-      </c>
-      <c r="I8" s="6">
-        <v>60</v>
-      </c>
-      <c r="J8" s="6">
-        <v>60</v>
+      <c r="G8" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="H8" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="I8" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="J8" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
       </c>
       <c r="K8" s="8"/>
     </row>
@@ -2241,17 +2285,21 @@
       <c r="F9" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="6">
-        <v>60</v>
-      </c>
-      <c r="H9" s="6">
-        <v>60</v>
-      </c>
-      <c r="I9" s="6">
-        <v>60</v>
-      </c>
-      <c r="J9" s="6">
-        <v>60</v>
+      <c r="G9" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H9" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="I9" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="J9" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>72</v>
       </c>
       <c r="K9" s="8"/>
     </row>
@@ -2274,17 +2322,21 @@
       <c r="F10" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="6">
-        <v>60</v>
-      </c>
-      <c r="H10" s="6">
-        <v>60</v>
-      </c>
-      <c r="I10" s="6">
-        <v>60</v>
-      </c>
-      <c r="J10" s="6">
-        <v>60</v>
+      <c r="G10" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="H10" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>95</v>
+      </c>
+      <c r="I10" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>87</v>
+      </c>
+      <c r="J10" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>77</v>
       </c>
       <c r="K10" s="8"/>
     </row>
@@ -2307,17 +2359,21 @@
       <c r="F11" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="6">
-        <v>60</v>
-      </c>
-      <c r="H11" s="6">
-        <v>60</v>
-      </c>
-      <c r="I11" s="6">
-        <v>60</v>
-      </c>
-      <c r="J11" s="6">
-        <v>60</v>
+      <c r="G11" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>99</v>
+      </c>
+      <c r="H11" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="I11" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="J11" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>62</v>
       </c>
       <c r="K11" s="8"/>
     </row>
@@ -2340,17 +2396,21 @@
       <c r="F12" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G12" s="6">
-        <v>60</v>
-      </c>
-      <c r="H12" s="6">
-        <v>60</v>
-      </c>
-      <c r="I12" s="6">
-        <v>60</v>
-      </c>
-      <c r="J12" s="6">
-        <v>60</v>
+      <c r="G12" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>97</v>
+      </c>
+      <c r="H12" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="I12" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="J12" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
       </c>
       <c r="K12" s="8"/>
     </row>
@@ -2373,17 +2433,21 @@
       <c r="F13" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G13" s="6">
-        <v>60</v>
-      </c>
-      <c r="H13" s="6">
-        <v>60</v>
-      </c>
-      <c r="I13" s="6">
-        <v>60</v>
-      </c>
-      <c r="J13" s="6">
-        <v>60</v>
+      <c r="G13" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>56</v>
+      </c>
+      <c r="H13" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="I13" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="J13" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>52</v>
       </c>
       <c r="K13" s="8"/>
     </row>
@@ -2406,17 +2470,21 @@
       <c r="F14" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="6">
-        <v>60</v>
-      </c>
-      <c r="H14" s="6">
-        <v>60</v>
-      </c>
-      <c r="I14" s="6">
-        <v>60</v>
-      </c>
-      <c r="J14" s="6">
-        <v>60</v>
+      <c r="G14" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="H14" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>79</v>
+      </c>
+      <c r="I14" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J14" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>49</v>
       </c>
       <c r="K14" s="8"/>
     </row>
@@ -2439,17 +2507,21 @@
       <c r="F15" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G15" s="6">
-        <v>60</v>
-      </c>
-      <c r="H15" s="6">
-        <v>60</v>
-      </c>
-      <c r="I15" s="6">
-        <v>60</v>
-      </c>
-      <c r="J15" s="6">
-        <v>60</v>
+      <c r="G15" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="H15" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="I15" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="J15" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>21</v>
       </c>
       <c r="K15" s="8"/>
     </row>
@@ -2472,17 +2544,21 @@
       <c r="F16" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G16" s="6">
-        <v>60</v>
-      </c>
-      <c r="H16" s="6">
-        <v>60</v>
-      </c>
-      <c r="I16" s="6">
-        <v>60</v>
-      </c>
-      <c r="J16" s="6">
-        <v>60</v>
+      <c r="G16" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="H16" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>82</v>
+      </c>
+      <c r="I16" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="J16" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>47</v>
       </c>
       <c r="K16" s="8"/>
     </row>
@@ -2505,17 +2581,21 @@
       <c r="F17" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G17" s="6">
-        <v>60</v>
-      </c>
-      <c r="H17" s="6">
-        <v>60</v>
-      </c>
-      <c r="I17" s="6">
-        <v>60</v>
-      </c>
-      <c r="J17" s="6">
-        <v>60</v>
+      <c r="G17" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="H17" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="I17" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="J17" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>38</v>
       </c>
       <c r="K17" s="8"/>
     </row>
@@ -2538,17 +2618,21 @@
       <c r="F18" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G18" s="6">
-        <v>60</v>
-      </c>
-      <c r="H18" s="6">
-        <v>60</v>
-      </c>
-      <c r="I18" s="6">
-        <v>60</v>
-      </c>
-      <c r="J18" s="6">
-        <v>60</v>
+      <c r="G18" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>82</v>
+      </c>
+      <c r="H18" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="I18" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="J18" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
       </c>
       <c r="K18" s="8"/>
     </row>
@@ -2571,17 +2655,21 @@
       <c r="F19" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G19" s="6">
-        <v>60</v>
-      </c>
-      <c r="H19" s="6">
-        <v>60</v>
-      </c>
-      <c r="I19" s="6">
-        <v>60</v>
-      </c>
-      <c r="J19" s="6">
-        <v>60</v>
+      <c r="G19" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="H19" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>94</v>
+      </c>
+      <c r="I19" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>85</v>
+      </c>
+      <c r="J19" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>23</v>
       </c>
       <c r="K19" s="8"/>
     </row>
@@ -2604,17 +2692,21 @@
       <c r="F20" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G20" s="6">
-        <v>60</v>
-      </c>
-      <c r="H20" s="6">
-        <v>60</v>
-      </c>
-      <c r="I20" s="6">
-        <v>60</v>
-      </c>
-      <c r="J20" s="6">
-        <v>60</v>
+      <c r="G20" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="H20" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="I20" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>91</v>
+      </c>
+      <c r="J20" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>11</v>
       </c>
       <c r="K20" s="8"/>
     </row>
@@ -2637,17 +2729,21 @@
       <c r="F21" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G21" s="6">
-        <v>60</v>
-      </c>
-      <c r="H21" s="6">
-        <v>60</v>
-      </c>
-      <c r="I21" s="6">
-        <v>60</v>
-      </c>
-      <c r="J21" s="6">
-        <v>60</v>
+      <c r="G21" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="H21" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="I21" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>93</v>
+      </c>
+      <c r="J21" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>70</v>
       </c>
       <c r="K21" s="8"/>
     </row>
@@ -2670,17 +2766,21 @@
       <c r="F22" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G22" s="6">
-        <v>60</v>
-      </c>
-      <c r="H22" s="6">
-        <v>60</v>
-      </c>
-      <c r="I22" s="6">
-        <v>60</v>
-      </c>
-      <c r="J22" s="6">
-        <v>60</v>
+      <c r="G22" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="H22" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>81</v>
+      </c>
+      <c r="I22" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="J22" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>50</v>
       </c>
       <c r="K22" s="8"/>
     </row>
@@ -2703,17 +2803,21 @@
       <c r="F23" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G23" s="6">
-        <v>60</v>
-      </c>
-      <c r="H23" s="6">
-        <v>60</v>
-      </c>
-      <c r="I23" s="6">
-        <v>60</v>
-      </c>
-      <c r="J23" s="6">
-        <v>60</v>
+      <c r="G23" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="H23" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="I23" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>79</v>
+      </c>
+      <c r="J23" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>33</v>
       </c>
       <c r="K23" s="8"/>
     </row>
@@ -2736,17 +2840,21 @@
       <c r="F24" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G24" s="6">
-        <v>60</v>
-      </c>
-      <c r="H24" s="6">
-        <v>60</v>
-      </c>
-      <c r="I24" s="6">
-        <v>60</v>
-      </c>
-      <c r="J24" s="6">
-        <v>60</v>
+      <c r="G24" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>92</v>
+      </c>
+      <c r="H24" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="I24" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="J24" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>81</v>
       </c>
       <c r="K24" s="8"/>
     </row>
@@ -2769,17 +2877,21 @@
       <c r="F25" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G25" s="6">
-        <v>60</v>
-      </c>
-      <c r="H25" s="6">
-        <v>60</v>
-      </c>
-      <c r="I25" s="6">
-        <v>60</v>
-      </c>
-      <c r="J25" s="6">
-        <v>60</v>
+      <c r="G25" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="H25" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="I25" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="J25" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>87</v>
       </c>
       <c r="K25" s="8"/>
     </row>
@@ -2802,17 +2914,21 @@
       <c r="F26" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G26" s="6">
-        <v>60</v>
-      </c>
-      <c r="H26" s="6">
-        <v>60</v>
-      </c>
-      <c r="I26" s="6">
-        <v>60</v>
-      </c>
-      <c r="J26" s="6">
-        <v>60</v>
+      <c r="G26" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="H26" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>96</v>
+      </c>
+      <c r="I26" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="J26" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>32</v>
       </c>
       <c r="K26" s="8"/>
     </row>
@@ -2835,17 +2951,21 @@
       <c r="F27" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G27" s="6">
+      <c r="G27" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="H27" s="9">
+        <f t="shared" ca="1" si="1"/>
         <v>60</v>
       </c>
-      <c r="H27" s="6">
-        <v>60</v>
-      </c>
-      <c r="I27" s="6">
-        <v>60</v>
-      </c>
-      <c r="J27" s="6">
-        <v>60</v>
+      <c r="I27" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="J27" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>67</v>
       </c>
       <c r="K27" s="8"/>
     </row>
@@ -2868,17 +2988,21 @@
       <c r="F28" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G28" s="6">
-        <v>60</v>
-      </c>
-      <c r="H28" s="6">
-        <v>60</v>
-      </c>
-      <c r="I28" s="6">
-        <v>60</v>
-      </c>
-      <c r="J28" s="6">
-        <v>60</v>
+      <c r="G28" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>77</v>
+      </c>
+      <c r="H28" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="I28" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="J28" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>36</v>
       </c>
       <c r="K28" s="8"/>
     </row>
@@ -2901,17 +3025,21 @@
       <c r="F29" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G29" s="6">
-        <v>60</v>
-      </c>
-      <c r="H29" s="6">
-        <v>60</v>
-      </c>
-      <c r="I29" s="6">
-        <v>60</v>
-      </c>
-      <c r="J29" s="6">
-        <v>60</v>
+      <c r="G29" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>95</v>
+      </c>
+      <c r="H29" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="I29" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="J29" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>20</v>
       </c>
       <c r="K29" s="8"/>
     </row>
@@ -2934,17 +3062,21 @@
       <c r="F30" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G30" s="6">
-        <v>60</v>
-      </c>
-      <c r="H30" s="6">
-        <v>60</v>
-      </c>
-      <c r="I30" s="6">
-        <v>60</v>
-      </c>
-      <c r="J30" s="6">
-        <v>60</v>
+      <c r="G30" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="H30" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="I30" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="J30" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>80</v>
       </c>
       <c r="K30" s="8"/>
     </row>
@@ -2967,17 +3099,21 @@
       <c r="F31" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G31" s="6">
-        <v>60</v>
-      </c>
-      <c r="H31" s="6">
-        <v>60</v>
-      </c>
-      <c r="I31" s="6">
-        <v>60</v>
-      </c>
-      <c r="J31" s="6">
-        <v>60</v>
+      <c r="G31" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="H31" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="I31" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="J31" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>41</v>
       </c>
       <c r="K31" s="8"/>
     </row>
@@ -3000,17 +3136,21 @@
       <c r="F32" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G32" s="6">
-        <v>60</v>
-      </c>
-      <c r="H32" s="6">
-        <v>60</v>
-      </c>
-      <c r="I32" s="6">
-        <v>60</v>
-      </c>
-      <c r="J32" s="6">
-        <v>60</v>
+      <c r="G32" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="H32" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="I32" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="J32" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>91</v>
       </c>
       <c r="K32" s="8"/>
     </row>
@@ -3033,17 +3173,21 @@
       <c r="F33" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G33" s="6">
-        <v>60</v>
-      </c>
-      <c r="H33" s="6">
-        <v>60</v>
-      </c>
-      <c r="I33" s="6">
-        <v>60</v>
-      </c>
-      <c r="J33" s="6">
-        <v>60</v>
+      <c r="G33" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="H33" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>56</v>
+      </c>
+      <c r="I33" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>94</v>
+      </c>
+      <c r="J33" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>19</v>
       </c>
       <c r="K33" s="8"/>
     </row>
@@ -3066,17 +3210,21 @@
       <c r="F34" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G34" s="6">
-        <v>60</v>
-      </c>
-      <c r="H34" s="6">
-        <v>60</v>
-      </c>
-      <c r="I34" s="6">
-        <v>60</v>
-      </c>
-      <c r="J34" s="6">
-        <v>60</v>
+      <c r="G34" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>91</v>
+      </c>
+      <c r="H34" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I34" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="J34" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>16</v>
       </c>
       <c r="K34" s="8"/>
     </row>
@@ -3099,17 +3247,21 @@
       <c r="F35" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G35" s="6">
-        <v>60</v>
-      </c>
-      <c r="H35" s="6">
-        <v>60</v>
-      </c>
-      <c r="I35" s="6">
-        <v>60</v>
-      </c>
-      <c r="J35" s="6">
-        <v>60</v>
+      <c r="G35" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="H35" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I35" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>78</v>
+      </c>
+      <c r="J35" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>38</v>
       </c>
       <c r="K35" s="8"/>
     </row>
@@ -3132,17 +3284,21 @@
       <c r="F36" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G36" s="6">
-        <v>60</v>
-      </c>
-      <c r="H36" s="6">
-        <v>60</v>
-      </c>
-      <c r="I36" s="6">
-        <v>60</v>
-      </c>
-      <c r="J36" s="6">
-        <v>60</v>
+      <c r="G36" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>76</v>
+      </c>
+      <c r="H36" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="I36" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="J36" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
       </c>
       <c r="K36" s="8"/>
     </row>
@@ -3165,17 +3321,21 @@
       <c r="F37" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G37" s="6">
-        <v>60</v>
-      </c>
-      <c r="H37" s="6">
-        <v>60</v>
-      </c>
-      <c r="I37" s="6">
-        <v>60</v>
-      </c>
-      <c r="J37" s="6">
-        <v>60</v>
+      <c r="G37" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="H37" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>59</v>
+      </c>
+      <c r="I37" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>85</v>
+      </c>
+      <c r="J37" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>88</v>
       </c>
       <c r="K37" s="8"/>
     </row>
@@ -3198,17 +3358,21 @@
       <c r="F38" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G38" s="6">
-        <v>60</v>
-      </c>
-      <c r="H38" s="6">
-        <v>60</v>
-      </c>
-      <c r="I38" s="6">
-        <v>60</v>
-      </c>
-      <c r="J38" s="6">
-        <v>60</v>
+      <c r="G38" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>91</v>
+      </c>
+      <c r="H38" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="I38" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>61</v>
+      </c>
+      <c r="J38" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>63</v>
       </c>
       <c r="K38" s="8"/>
     </row>
@@ -3231,17 +3395,21 @@
       <c r="F39" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G39" s="6">
-        <v>60</v>
-      </c>
-      <c r="H39" s="6">
-        <v>60</v>
-      </c>
-      <c r="I39" s="6">
-        <v>60</v>
-      </c>
-      <c r="J39" s="6">
-        <v>60</v>
+      <c r="G39" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="H39" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="I39" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J39" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
       </c>
       <c r="K39" s="8"/>
     </row>
@@ -3264,17 +3432,21 @@
       <c r="F40" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G40" s="6">
-        <v>60</v>
-      </c>
-      <c r="H40" s="6">
-        <v>60</v>
-      </c>
-      <c r="I40" s="6">
-        <v>60</v>
-      </c>
-      <c r="J40" s="6">
-        <v>60</v>
+      <c r="G40" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="H40" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="I40" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="J40" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
       </c>
       <c r="K40" s="8"/>
     </row>
@@ -3297,17 +3469,21 @@
       <c r="F41" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G41" s="6">
-        <v>60</v>
-      </c>
-      <c r="H41" s="6">
-        <v>60</v>
-      </c>
-      <c r="I41" s="6">
-        <v>60</v>
-      </c>
-      <c r="J41" s="6">
-        <v>60</v>
+      <c r="G41" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="H41" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>87</v>
+      </c>
+      <c r="I41" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="J41" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>42</v>
       </c>
       <c r="K41" s="8"/>
     </row>
@@ -3330,17 +3506,21 @@
       <c r="F42" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G42" s="6">
-        <v>60</v>
-      </c>
-      <c r="H42" s="6">
-        <v>60</v>
-      </c>
-      <c r="I42" s="6">
-        <v>60</v>
-      </c>
-      <c r="J42" s="6">
-        <v>60</v>
+      <c r="G42" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>92</v>
+      </c>
+      <c r="H42" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>74</v>
+      </c>
+      <c r="I42" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>91</v>
+      </c>
+      <c r="J42" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>36</v>
       </c>
       <c r="K42" s="8"/>
     </row>
@@ -3363,17 +3543,21 @@
       <c r="F43" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G43" s="6">
-        <v>60</v>
-      </c>
-      <c r="H43" s="6">
-        <v>60</v>
-      </c>
-      <c r="I43" s="6">
-        <v>60</v>
-      </c>
-      <c r="J43" s="6">
-        <v>60</v>
+      <c r="G43" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="H43" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="I43" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="J43" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>31</v>
       </c>
       <c r="K43" s="8"/>
     </row>
@@ -3396,17 +3580,21 @@
       <c r="F44" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G44" s="6">
-        <v>60</v>
-      </c>
-      <c r="H44" s="6">
-        <v>60</v>
-      </c>
-      <c r="I44" s="6">
-        <v>60</v>
-      </c>
-      <c r="J44" s="6">
-        <v>60</v>
+      <c r="G44" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="H44" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>71</v>
+      </c>
+      <c r="I44" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="J44" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>21</v>
       </c>
       <c r="K44" s="8"/>
     </row>
@@ -3429,17 +3617,21 @@
       <c r="F45" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G45" s="6">
-        <v>60</v>
-      </c>
-      <c r="H45" s="6">
-        <v>60</v>
-      </c>
-      <c r="I45" s="6">
-        <v>60</v>
-      </c>
-      <c r="J45" s="6">
-        <v>60</v>
+      <c r="G45" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="H45" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="I45" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="J45" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>90</v>
       </c>
       <c r="K45" s="8"/>
     </row>
@@ -3462,17 +3654,21 @@
       <c r="F46" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G46" s="6">
-        <v>60</v>
-      </c>
-      <c r="H46" s="6">
-        <v>60</v>
-      </c>
-      <c r="I46" s="6">
-        <v>60</v>
-      </c>
-      <c r="J46" s="6">
-        <v>60</v>
+      <c r="G46" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>84</v>
+      </c>
+      <c r="H46" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="I46" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>92</v>
+      </c>
+      <c r="J46" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>59</v>
       </c>
       <c r="K46" s="8"/>
     </row>
@@ -3495,17 +3691,21 @@
       <c r="F47" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G47" s="6">
-        <v>60</v>
-      </c>
-      <c r="H47" s="6">
-        <v>60</v>
-      </c>
-      <c r="I47" s="6">
-        <v>60</v>
-      </c>
-      <c r="J47" s="6">
-        <v>60</v>
+      <c r="G47" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="H47" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="I47" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="J47" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>22</v>
       </c>
       <c r="K47" s="8"/>
     </row>
@@ -3528,17 +3728,21 @@
       <c r="F48" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G48" s="6">
-        <v>60</v>
-      </c>
-      <c r="H48" s="6">
-        <v>60</v>
-      </c>
-      <c r="I48" s="6">
-        <v>60</v>
-      </c>
-      <c r="J48" s="6">
-        <v>60</v>
+      <c r="G48" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="H48" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>62</v>
+      </c>
+      <c r="I48" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="J48" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>93</v>
       </c>
       <c r="K48" s="8"/>
     </row>
@@ -3561,17 +3765,21 @@
       <c r="F49" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G49" s="6">
-        <v>60</v>
-      </c>
-      <c r="H49" s="6">
-        <v>60</v>
-      </c>
-      <c r="I49" s="6">
-        <v>60</v>
-      </c>
-      <c r="J49" s="6">
-        <v>60</v>
+      <c r="G49" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="H49" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>53</v>
+      </c>
+      <c r="I49" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="J49" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>28</v>
       </c>
       <c r="K49" s="8"/>
     </row>
@@ -3594,17 +3802,21 @@
       <c r="F50" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G50" s="8">
-        <v>60</v>
-      </c>
-      <c r="H50" s="8">
-        <v>60</v>
-      </c>
-      <c r="I50" s="8">
-        <v>60</v>
-      </c>
-      <c r="J50" s="8">
-        <v>60</v>
+      <c r="G50" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="H50" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I50" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>85</v>
+      </c>
+      <c r="J50" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>99</v>
       </c>
       <c r="K50" s="8"/>
     </row>

</xml_diff>

<commit_message>
Made the data better.
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eren\Desktop\codes\Python\Django\ses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{816FA4A5-3022-4CA5-9E1C-04EEB36958F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D01971E9-6C7A-42D2-88C2-EAF80601CE23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -203,153 +203,6 @@
     <t>49</t>
   </si>
   <si>
-    <t>202400001</t>
-  </si>
-  <si>
-    <t>202400002</t>
-  </si>
-  <si>
-    <t>202400003</t>
-  </si>
-  <si>
-    <t>202400004</t>
-  </si>
-  <si>
-    <t>202400005</t>
-  </si>
-  <si>
-    <t>202400006</t>
-  </si>
-  <si>
-    <t>202400007</t>
-  </si>
-  <si>
-    <t>202400008</t>
-  </si>
-  <si>
-    <t>202400009</t>
-  </si>
-  <si>
-    <t>202400010</t>
-  </si>
-  <si>
-    <t>202400011</t>
-  </si>
-  <si>
-    <t>202400012</t>
-  </si>
-  <si>
-    <t>202400013</t>
-  </si>
-  <si>
-    <t>202400014</t>
-  </si>
-  <si>
-    <t>202400015</t>
-  </si>
-  <si>
-    <t>202400016</t>
-  </si>
-  <si>
-    <t>202400017</t>
-  </si>
-  <si>
-    <t>202400018</t>
-  </si>
-  <si>
-    <t>202400019</t>
-  </si>
-  <si>
-    <t>202400020</t>
-  </si>
-  <si>
-    <t>202400021</t>
-  </si>
-  <si>
-    <t>202400022</t>
-  </si>
-  <si>
-    <t>202400023</t>
-  </si>
-  <si>
-    <t>202400024</t>
-  </si>
-  <si>
-    <t>202400025</t>
-  </si>
-  <si>
-    <t>202400026</t>
-  </si>
-  <si>
-    <t>202400027</t>
-  </si>
-  <si>
-    <t>202400028</t>
-  </si>
-  <si>
-    <t>202400029</t>
-  </si>
-  <si>
-    <t>202400030</t>
-  </si>
-  <si>
-    <t>202400031</t>
-  </si>
-  <si>
-    <t>202400032</t>
-  </si>
-  <si>
-    <t>202400033</t>
-  </si>
-  <si>
-    <t>202400034</t>
-  </si>
-  <si>
-    <t>202400035</t>
-  </si>
-  <si>
-    <t>202400036</t>
-  </si>
-  <si>
-    <t>202400037</t>
-  </si>
-  <si>
-    <t>202400038</t>
-  </si>
-  <si>
-    <t>202400039</t>
-  </si>
-  <si>
-    <t>202400040</t>
-  </si>
-  <si>
-    <t>202400041</t>
-  </si>
-  <si>
-    <t>202400042</t>
-  </si>
-  <si>
-    <t>202400043</t>
-  </si>
-  <si>
-    <t>202400044</t>
-  </si>
-  <si>
-    <t>202400045</t>
-  </si>
-  <si>
-    <t>202400046</t>
-  </si>
-  <si>
-    <t>202400047</t>
-  </si>
-  <si>
-    <t>202400048</t>
-  </si>
-  <si>
-    <t>202400049</t>
-  </si>
-  <si>
     <t>Midterm(%25)_0833AB</t>
   </si>
   <si>
@@ -359,9 +212,6 @@
     <t>Final(%40)_0833AB</t>
   </si>
   <si>
-    <t>Homeworks(%10)_0833AB</t>
-  </si>
-  <si>
     <t>studentname1</t>
   </si>
   <si>
@@ -654,6 +504,156 @@
   </si>
   <si>
     <t>studentsurname49</t>
+  </si>
+  <si>
+    <t>Project(%10)_0833AB</t>
+  </si>
+  <si>
+    <t>202500001</t>
+  </si>
+  <si>
+    <t>202500002</t>
+  </si>
+  <si>
+    <t>202500003</t>
+  </si>
+  <si>
+    <t>202500004</t>
+  </si>
+  <si>
+    <t>202500005</t>
+  </si>
+  <si>
+    <t>202500006</t>
+  </si>
+  <si>
+    <t>202500007</t>
+  </si>
+  <si>
+    <t>202500008</t>
+  </si>
+  <si>
+    <t>202500009</t>
+  </si>
+  <si>
+    <t>202500010</t>
+  </si>
+  <si>
+    <t>202500011</t>
+  </si>
+  <si>
+    <t>202500012</t>
+  </si>
+  <si>
+    <t>202500013</t>
+  </si>
+  <si>
+    <t>202500014</t>
+  </si>
+  <si>
+    <t>202500015</t>
+  </si>
+  <si>
+    <t>202500016</t>
+  </si>
+  <si>
+    <t>202500017</t>
+  </si>
+  <si>
+    <t>202500018</t>
+  </si>
+  <si>
+    <t>202500019</t>
+  </si>
+  <si>
+    <t>202500020</t>
+  </si>
+  <si>
+    <t>202500021</t>
+  </si>
+  <si>
+    <t>202500022</t>
+  </si>
+  <si>
+    <t>202500023</t>
+  </si>
+  <si>
+    <t>202500024</t>
+  </si>
+  <si>
+    <t>202500025</t>
+  </si>
+  <si>
+    <t>202500026</t>
+  </si>
+  <si>
+    <t>202500027</t>
+  </si>
+  <si>
+    <t>202500028</t>
+  </si>
+  <si>
+    <t>202500029</t>
+  </si>
+  <si>
+    <t>202500030</t>
+  </si>
+  <si>
+    <t>202500031</t>
+  </si>
+  <si>
+    <t>202500032</t>
+  </si>
+  <si>
+    <t>202500033</t>
+  </si>
+  <si>
+    <t>202500034</t>
+  </si>
+  <si>
+    <t>202500035</t>
+  </si>
+  <si>
+    <t>202500036</t>
+  </si>
+  <si>
+    <t>202500037</t>
+  </si>
+  <si>
+    <t>202500038</t>
+  </si>
+  <si>
+    <t>202500039</t>
+  </si>
+  <si>
+    <t>202500040</t>
+  </si>
+  <si>
+    <t>202500041</t>
+  </si>
+  <si>
+    <t>202500042</t>
+  </si>
+  <si>
+    <t>202500043</t>
+  </si>
+  <si>
+    <t>202500044</t>
+  </si>
+  <si>
+    <t>202500045</t>
+  </si>
+  <si>
+    <t>202500046</t>
+  </si>
+  <si>
+    <t>202500047</t>
+  </si>
+  <si>
+    <t>202500048</t>
+  </si>
+  <si>
+    <t>202500049</t>
   </si>
 </sst>
 </file>
@@ -1952,8 +1952,8 @@
   </sheetPr>
   <dimension ref="A1:K60"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:J50"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:J50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1992,16 +1992,16 @@
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>105</v>
+        <v>56</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>106</v>
+        <v>57</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>108</v>
+        <v>157</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>107</v>
+        <v>58</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>6</v>
@@ -2012,13 +2012,13 @@
         <v>7</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>56</v>
+        <v>158</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>109</v>
+        <v>59</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>158</v>
+        <v>108</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>8</v>
@@ -2027,20 +2027,20 @@
         <v>7</v>
       </c>
       <c r="G2" s="9">
-        <f ca="1">TRUNC(RAND()*100)</f>
-        <v>34</v>
+        <f t="shared" ref="G2:I50" ca="1" si="0">TRUNC(60 + ((RAND()*100 - 0) * (100 - 60) / (100 - 0)))</f>
+        <v>68</v>
       </c>
       <c r="H2" s="9">
-        <f t="shared" ref="H2:J17" ca="1" si="0">TRUNC(RAND()*100)</f>
-        <v>96</v>
+        <f ca="1">TRUNC(60 + ((RAND()*100 - 0) * (100 - 60) / (100 - 0)))</f>
+        <v>79</v>
       </c>
       <c r="I2" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>64</v>
+        <f ca="1">TRUNC(30 + ((RAND()*100 - 0) * (60 - 30) / (100 - 0)))</f>
+        <v>40</v>
       </c>
       <c r="J2" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>38</v>
+        <f ca="1">TRUNC(30 + ((RAND()*100 - 0) * (60 - 30) / (100 - 0)))</f>
+        <v>36</v>
       </c>
       <c r="K2" s="6"/>
     </row>
@@ -2049,13 +2049,13 @@
         <v>9</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>57</v>
+        <v>159</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>159</v>
+        <v>109</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>8</v>
@@ -2064,20 +2064,20 @@
         <v>7</v>
       </c>
       <c r="G3" s="9">
-        <f t="shared" ref="G3:J50" ca="1" si="1">TRUNC(RAND()*100)</f>
-        <v>97</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>90</v>
       </c>
       <c r="H3" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>63</v>
       </c>
       <c r="I3" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>54</v>
+        <f t="shared" ref="I3:J50" ca="1" si="1">TRUNC(30 + ((RAND()*100 - 0) * (60 - 30) / (100 - 0)))</f>
+        <v>49</v>
       </c>
       <c r="J3" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>58</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>35</v>
       </c>
       <c r="K3" s="8"/>
     </row>
@@ -2086,13 +2086,13 @@
         <v>10</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>58</v>
+        <v>160</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>111</v>
+        <v>61</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>160</v>
+        <v>110</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>10</v>
@@ -2101,20 +2101,20 @@
         <v>7</v>
       </c>
       <c r="G4" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>30</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>68</v>
       </c>
       <c r="H4" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>68</v>
+        <v>96</v>
       </c>
       <c r="I4" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>59</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>47</v>
       </c>
       <c r="J4" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>95</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>39</v>
       </c>
       <c r="K4" s="8"/>
     </row>
@@ -2123,13 +2123,13 @@
         <v>8</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>59</v>
+        <v>161</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>112</v>
+        <v>62</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>161</v>
+        <v>111</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>10</v>
@@ -2138,20 +2138,20 @@
         <v>7</v>
       </c>
       <c r="G5" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>51</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>72</v>
       </c>
       <c r="H5" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+        <v>92</v>
       </c>
       <c r="I5" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>68</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>41</v>
       </c>
       <c r="J5" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>76</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>44</v>
       </c>
       <c r="K5" s="8"/>
     </row>
@@ -2160,13 +2160,13 @@
         <v>11</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>60</v>
+        <v>162</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>113</v>
+        <v>63</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>162</v>
+        <v>112</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>8</v>
@@ -2175,20 +2175,20 @@
         <v>7</v>
       </c>
       <c r="G6" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>88</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>75</v>
       </c>
       <c r="H6" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <v>60</v>
       </c>
       <c r="I6" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>99</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>32</v>
       </c>
       <c r="J6" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>46</v>
       </c>
       <c r="K6" s="8"/>
     </row>
@@ -2197,13 +2197,13 @@
         <v>12</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>61</v>
+        <v>163</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>114</v>
+        <v>64</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>163</v>
+        <v>113</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>10</v>
@@ -2212,20 +2212,20 @@
         <v>7</v>
       </c>
       <c r="G7" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>34</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>84</v>
       </c>
       <c r="H7" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="I7" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>67</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>55</v>
       </c>
       <c r="J7" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>31</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>51</v>
       </c>
       <c r="K7" s="8"/>
     </row>
@@ -2234,13 +2234,13 @@
         <v>13</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>62</v>
+        <v>164</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>115</v>
+        <v>65</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>164</v>
+        <v>114</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>10</v>
@@ -2249,20 +2249,20 @@
         <v>7</v>
       </c>
       <c r="G8" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>14</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>92</v>
       </c>
       <c r="H8" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>45</v>
+        <v>87</v>
       </c>
       <c r="I8" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>43</v>
       </c>
       <c r="J8" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>42</v>
       </c>
       <c r="K8" s="8"/>
     </row>
@@ -2271,13 +2271,13 @@
         <v>14</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>63</v>
+        <v>165</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>116</v>
+        <v>66</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>165</v>
+        <v>115</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>10</v>
@@ -2286,20 +2286,20 @@
         <v>7</v>
       </c>
       <c r="G9" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>73</v>
       </c>
       <c r="H9" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+        <v>74</v>
       </c>
       <c r="I9" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>66</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>44</v>
       </c>
       <c r="J9" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>72</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>48</v>
       </c>
       <c r="K9" s="8"/>
     </row>
@@ -2308,13 +2308,13 @@
         <v>15</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>64</v>
+        <v>166</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>117</v>
+        <v>67</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>166</v>
+        <v>116</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>10</v>
@@ -2323,20 +2323,20 @@
         <v>7</v>
       </c>
       <c r="G10" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>70</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>68</v>
       </c>
       <c r="H10" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="I10" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>87</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>43</v>
       </c>
       <c r="J10" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>77</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>52</v>
       </c>
       <c r="K10" s="8"/>
     </row>
@@ -2345,13 +2345,13 @@
         <v>16</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>65</v>
+        <v>167</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>118</v>
+        <v>68</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>167</v>
+        <v>117</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>10</v>
@@ -2360,20 +2360,20 @@
         <v>7</v>
       </c>
       <c r="G11" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>99</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>92</v>
       </c>
       <c r="H11" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="I11" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>32</v>
       </c>
       <c r="J11" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>62</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>37</v>
       </c>
       <c r="K11" s="8"/>
     </row>
@@ -2382,13 +2382,13 @@
         <v>17</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>66</v>
+        <v>168</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>119</v>
+        <v>69</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>168</v>
+        <v>118</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>10</v>
@@ -2397,20 +2397,20 @@
         <v>7</v>
       </c>
       <c r="G12" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>97</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>72</v>
       </c>
       <c r="H12" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>60</v>
       </c>
       <c r="I12" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>69</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>48</v>
       </c>
       <c r="J12" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>34</v>
       </c>
       <c r="K12" s="8"/>
     </row>
@@ -2419,13 +2419,13 @@
         <v>18</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>67</v>
+        <v>169</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>120</v>
+        <v>70</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>169</v>
+        <v>119</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>10</v>
@@ -2434,19 +2434,19 @@
         <v>7</v>
       </c>
       <c r="G13" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>56</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>70</v>
       </c>
       <c r="H13" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="I13" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>56</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>54</v>
       </c>
       <c r="J13" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>52</v>
       </c>
       <c r="K13" s="8"/>
@@ -2456,13 +2456,13 @@
         <v>19</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>68</v>
+        <v>170</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>121</v>
+        <v>71</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>170</v>
+        <v>120</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>10</v>
@@ -2471,20 +2471,20 @@
         <v>7</v>
       </c>
       <c r="G14" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>55</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>98</v>
       </c>
       <c r="H14" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="I14" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>54</v>
       </c>
       <c r="J14" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>49</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>32</v>
       </c>
       <c r="K14" s="8"/>
     </row>
@@ -2493,13 +2493,13 @@
         <v>20</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>69</v>
+        <v>171</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>122</v>
+        <v>72</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>171</v>
+        <v>121</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>10</v>
@@ -2508,20 +2508,20 @@
         <v>7</v>
       </c>
       <c r="G15" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>14</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>63</v>
       </c>
       <c r="H15" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="I15" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>30</v>
       </c>
       <c r="J15" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>57</v>
       </c>
       <c r="K15" s="8"/>
     </row>
@@ -2530,35 +2530,35 @@
         <v>21</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" s="9">
+        <f t="shared" ca="1" si="0"/>
         <v>70</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G16" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>14</v>
-      </c>
       <c r="H16" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="I16" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>50</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>43</v>
       </c>
       <c r="J16" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>47</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>31</v>
       </c>
       <c r="K16" s="8"/>
     </row>
@@ -2567,13 +2567,13 @@
         <v>22</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>71</v>
+        <v>173</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>124</v>
+        <v>74</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>173</v>
+        <v>123</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>10</v>
@@ -2582,20 +2582,20 @@
         <v>7</v>
       </c>
       <c r="G17" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>23</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>82</v>
       </c>
       <c r="H17" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="I17" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>58</v>
       </c>
       <c r="J17" s="9">
-        <f t="shared" ca="1" si="0"/>
-        <v>38</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>54</v>
       </c>
       <c r="K17" s="8"/>
     </row>
@@ -2604,13 +2604,13 @@
         <v>23</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>72</v>
+        <v>174</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>125</v>
+        <v>75</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>174</v>
+        <v>124</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>8</v>
@@ -2619,20 +2619,20 @@
         <v>7</v>
       </c>
       <c r="G18" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>82</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>85</v>
       </c>
       <c r="H18" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>36</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>85</v>
       </c>
       <c r="I18" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="J18" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="K18" s="8"/>
     </row>
@@ -2641,13 +2641,13 @@
         <v>24</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>73</v>
+        <v>175</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>126</v>
+        <v>76</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>175</v>
+        <v>125</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>10</v>
@@ -2656,20 +2656,20 @@
         <v>7</v>
       </c>
       <c r="G19" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>38</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>87</v>
       </c>
       <c r="H19" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>94</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>82</v>
       </c>
       <c r="I19" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>85</v>
+        <v>59</v>
       </c>
       <c r="J19" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="K19" s="8"/>
     </row>
@@ -2678,13 +2678,13 @@
         <v>25</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>74</v>
+        <v>176</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>127</v>
+        <v>77</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>176</v>
+        <v>126</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>10</v>
@@ -2693,20 +2693,20 @@
         <v>7</v>
       </c>
       <c r="G20" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>24</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>64</v>
       </c>
       <c r="H20" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>77</v>
       </c>
       <c r="I20" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>91</v>
+        <v>36</v>
       </c>
       <c r="J20" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="K20" s="8"/>
     </row>
@@ -2715,13 +2715,13 @@
         <v>26</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>75</v>
+        <v>177</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>128</v>
+        <v>78</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>177</v>
+        <v>127</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>10</v>
@@ -2730,20 +2730,20 @@
         <v>7</v>
       </c>
       <c r="G21" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>87</v>
       </c>
       <c r="H21" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>28</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>69</v>
       </c>
       <c r="I21" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>93</v>
+        <v>55</v>
       </c>
       <c r="J21" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>70</v>
+        <v>41</v>
       </c>
       <c r="K21" s="8"/>
     </row>
@@ -2752,13 +2752,13 @@
         <v>27</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>76</v>
+        <v>178</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>129</v>
+        <v>79</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>178</v>
+        <v>128</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>8</v>
@@ -2767,20 +2767,20 @@
         <v>7</v>
       </c>
       <c r="G22" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>64</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>81</v>
       </c>
       <c r="H22" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>81</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>73</v>
       </c>
       <c r="I22" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="J22" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="K22" s="8"/>
     </row>
@@ -2789,13 +2789,13 @@
         <v>28</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>77</v>
+        <v>179</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>179</v>
+        <v>129</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>10</v>
@@ -2804,20 +2804,20 @@
         <v>7</v>
       </c>
       <c r="G23" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>23</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>60</v>
       </c>
       <c r="H23" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>21</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>66</v>
       </c>
       <c r="I23" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="J23" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K23" s="8"/>
     </row>
@@ -2826,13 +2826,13 @@
         <v>29</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>78</v>
+        <v>180</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>131</v>
+        <v>81</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>180</v>
+        <v>130</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>10</v>
@@ -2841,20 +2841,20 @@
         <v>7</v>
       </c>
       <c r="G24" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>92</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>85</v>
       </c>
       <c r="H24" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>36</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>86</v>
       </c>
       <c r="I24" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="J24" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>81</v>
+        <v>38</v>
       </c>
       <c r="K24" s="8"/>
     </row>
@@ -2863,13 +2863,13 @@
         <v>30</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>79</v>
+        <v>181</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>132</v>
+        <v>82</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>181</v>
+        <v>131</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>10</v>
@@ -2878,20 +2878,20 @@
         <v>7</v>
       </c>
       <c r="G25" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>90</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>75</v>
       </c>
       <c r="H25" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>14</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>87</v>
       </c>
       <c r="I25" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="J25" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>87</v>
+        <v>32</v>
       </c>
       <c r="K25" s="8"/>
     </row>
@@ -2900,13 +2900,13 @@
         <v>31</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>80</v>
+        <v>182</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>133</v>
+        <v>83</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>10</v>
@@ -2915,20 +2915,20 @@
         <v>7</v>
       </c>
       <c r="G26" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>38</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>81</v>
       </c>
       <c r="H26" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>96</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>95</v>
       </c>
       <c r="I26" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="J26" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K26" s="8"/>
     </row>
@@ -2937,13 +2937,13 @@
         <v>32</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>81</v>
+        <v>183</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>134</v>
+        <v>84</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>10</v>
@@ -2952,20 +2952,20 @@
         <v>7</v>
       </c>
       <c r="G27" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>45</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>77</v>
       </c>
       <c r="H27" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>60</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>98</v>
       </c>
       <c r="I27" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="J27" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="K27" s="8"/>
     </row>
@@ -2974,13 +2974,13 @@
         <v>33</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>82</v>
+        <v>184</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>135</v>
+        <v>85</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>184</v>
+        <v>134</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>10</v>
@@ -2989,20 +2989,20 @@
         <v>7</v>
       </c>
       <c r="G28" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>77</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>96</v>
       </c>
       <c r="H28" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>22</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>79</v>
       </c>
       <c r="I28" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="J28" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="K28" s="8"/>
     </row>
@@ -3011,13 +3011,13 @@
         <v>34</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>83</v>
+        <v>185</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>136</v>
+        <v>86</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>185</v>
+        <v>135</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>10</v>
@@ -3026,20 +3026,20 @@
         <v>7</v>
       </c>
       <c r="G29" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>95</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>84</v>
       </c>
       <c r="H29" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>23</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>88</v>
       </c>
       <c r="I29" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="J29" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="K29" s="8"/>
     </row>
@@ -3048,13 +3048,13 @@
         <v>35</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>84</v>
+        <v>186</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>137</v>
+        <v>87</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>186</v>
+        <v>136</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>10</v>
@@ -3063,20 +3063,20 @@
         <v>7</v>
       </c>
       <c r="G30" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>14</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>95</v>
       </c>
       <c r="H30" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>23</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>78</v>
       </c>
       <c r="I30" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J30" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>80</v>
+        <v>38</v>
       </c>
       <c r="K30" s="8"/>
     </row>
@@ -3085,13 +3085,13 @@
         <v>36</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>85</v>
+        <v>187</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>138</v>
+        <v>88</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>187</v>
+        <v>137</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>10</v>
@@ -3100,20 +3100,20 @@
         <v>7</v>
       </c>
       <c r="G31" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>79</v>
+      </c>
+      <c r="H31" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="I31" s="9">
         <f t="shared" ca="1" si="1"/>
         <v>33</v>
       </c>
-      <c r="H31" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>75</v>
-      </c>
-      <c r="I31" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>15</v>
-      </c>
       <c r="J31" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="K31" s="8"/>
     </row>
@@ -3122,13 +3122,13 @@
         <v>37</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>86</v>
+        <v>188</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>139</v>
+        <v>89</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>188</v>
+        <v>138</v>
       </c>
       <c r="E32" s="7" t="s">
         <v>10</v>
@@ -3137,20 +3137,20 @@
         <v>7</v>
       </c>
       <c r="G32" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>72</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>95</v>
       </c>
       <c r="H32" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>80</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>83</v>
       </c>
       <c r="I32" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>58</v>
       </c>
       <c r="J32" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>91</v>
+        <v>46</v>
       </c>
       <c r="K32" s="8"/>
     </row>
@@ -3159,13 +3159,13 @@
         <v>38</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>87</v>
+        <v>189</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>140</v>
+        <v>90</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>189</v>
+        <v>139</v>
       </c>
       <c r="E33" s="7" t="s">
         <v>10</v>
@@ -3174,20 +3174,20 @@
         <v>7</v>
       </c>
       <c r="G33" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>72</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>90</v>
       </c>
       <c r="H33" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>56</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>99</v>
       </c>
       <c r="I33" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>94</v>
+        <v>42</v>
       </c>
       <c r="J33" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="K33" s="8"/>
     </row>
@@ -3196,13 +3196,13 @@
         <v>39</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>88</v>
+        <v>190</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>141</v>
+        <v>91</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>190</v>
+        <v>140</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>10</v>
@@ -3211,20 +3211,20 @@
         <v>7</v>
       </c>
       <c r="G34" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>91</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>70</v>
       </c>
       <c r="H34" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>82</v>
       </c>
       <c r="I34" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="J34" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="K34" s="8"/>
     </row>
@@ -3233,13 +3233,13 @@
         <v>40</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>89</v>
+        <v>191</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>142</v>
+        <v>92</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>191</v>
+        <v>141</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>10</v>
@@ -3248,20 +3248,20 @@
         <v>7</v>
       </c>
       <c r="G35" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>27</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>60</v>
       </c>
       <c r="H35" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>50</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>82</v>
       </c>
       <c r="I35" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>78</v>
+        <v>37</v>
       </c>
       <c r="J35" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="K35" s="8"/>
     </row>
@@ -3270,13 +3270,13 @@
         <v>41</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>90</v>
+        <v>192</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>143</v>
+        <v>93</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>192</v>
+        <v>142</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>10</v>
@@ -3285,20 +3285,20 @@
         <v>7</v>
       </c>
       <c r="G36" s="9">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
+        <v>92</v>
+      </c>
+      <c r="H36" s="9">
+        <f t="shared" ca="1" si="0"/>
         <v>76</v>
       </c>
-      <c r="H36" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>3</v>
-      </c>
       <c r="I36" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="J36" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="K36" s="8"/>
     </row>
@@ -3307,13 +3307,13 @@
         <v>42</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>91</v>
+        <v>193</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>144</v>
+        <v>94</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>193</v>
+        <v>143</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>10</v>
@@ -3322,20 +3322,20 @@
         <v>7</v>
       </c>
       <c r="G37" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>41</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>76</v>
       </c>
       <c r="H37" s="9">
+        <f t="shared" ca="1" si="0"/>
+        <v>78</v>
+      </c>
+      <c r="I37" s="9">
+        <f t="shared" ca="1" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="J37" s="9">
         <f t="shared" ca="1" si="1"/>
         <v>59</v>
-      </c>
-      <c r="I37" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>85</v>
-      </c>
-      <c r="J37" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>88</v>
       </c>
       <c r="K37" s="8"/>
     </row>
@@ -3344,13 +3344,13 @@
         <v>43</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>92</v>
+        <v>194</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>145</v>
+        <v>95</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>194</v>
+        <v>144</v>
       </c>
       <c r="E38" s="7" t="s">
         <v>10</v>
@@ -3359,20 +3359,20 @@
         <v>7</v>
       </c>
       <c r="G38" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>91</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>66</v>
       </c>
       <c r="H38" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>72</v>
       </c>
       <c r="I38" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="J38" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="K38" s="8"/>
     </row>
@@ -3381,13 +3381,13 @@
         <v>44</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>93</v>
+        <v>195</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>146</v>
+        <v>96</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>195</v>
+        <v>145</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>10</v>
@@ -3396,20 +3396,20 @@
         <v>7</v>
       </c>
       <c r="G39" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>44</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>78</v>
       </c>
       <c r="H39" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>47</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>90</v>
       </c>
       <c r="I39" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="J39" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="K39" s="8"/>
     </row>
@@ -3418,13 +3418,13 @@
         <v>45</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>94</v>
+        <v>196</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>147</v>
+        <v>97</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>196</v>
+        <v>146</v>
       </c>
       <c r="E40" s="7" t="s">
         <v>10</v>
@@ -3433,20 +3433,20 @@
         <v>7</v>
       </c>
       <c r="G40" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>51</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>85</v>
       </c>
       <c r="H40" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>37</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>77</v>
       </c>
       <c r="I40" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="J40" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="K40" s="8"/>
     </row>
@@ -3455,13 +3455,13 @@
         <v>46</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>95</v>
+        <v>197</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>148</v>
+        <v>98</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>197</v>
+        <v>147</v>
       </c>
       <c r="E41" s="7" t="s">
         <v>10</v>
@@ -3470,20 +3470,20 @@
         <v>7</v>
       </c>
       <c r="G41" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>30</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>75</v>
       </c>
       <c r="H41" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>87</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>93</v>
       </c>
       <c r="I41" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="J41" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="K41" s="8"/>
     </row>
@@ -3492,13 +3492,13 @@
         <v>47</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>96</v>
+        <v>198</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>149</v>
+        <v>99</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>198</v>
+        <v>148</v>
       </c>
       <c r="E42" s="7" t="s">
         <v>10</v>
@@ -3507,20 +3507,20 @@
         <v>7</v>
       </c>
       <c r="G42" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>92</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>99</v>
       </c>
       <c r="H42" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>74</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>89</v>
       </c>
       <c r="I42" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>91</v>
+        <v>57</v>
       </c>
       <c r="J42" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="K42" s="8"/>
     </row>
@@ -3529,13 +3529,13 @@
         <v>48</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>97</v>
+        <v>199</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>199</v>
+        <v>149</v>
       </c>
       <c r="E43" s="7" t="s">
         <v>10</v>
@@ -3544,20 +3544,20 @@
         <v>7</v>
       </c>
       <c r="G43" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>64</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>80</v>
       </c>
       <c r="H43" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>26</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>95</v>
       </c>
       <c r="I43" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="J43" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="K43" s="8"/>
     </row>
@@ -3566,13 +3566,13 @@
         <v>49</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>98</v>
+        <v>200</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>151</v>
+        <v>101</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="E44" s="7" t="s">
         <v>10</v>
@@ -3581,20 +3581,20 @@
         <v>7</v>
       </c>
       <c r="G44" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>73</v>
       </c>
       <c r="H44" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>71</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>78</v>
       </c>
       <c r="I44" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J44" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="K44" s="8"/>
     </row>
@@ -3603,13 +3603,13 @@
         <v>50</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>99</v>
+        <v>201</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>152</v>
+        <v>102</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>201</v>
+        <v>151</v>
       </c>
       <c r="E45" s="7" t="s">
         <v>10</v>
@@ -3618,20 +3618,20 @@
         <v>7</v>
       </c>
       <c r="G45" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>80</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>89</v>
       </c>
       <c r="H45" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>22</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>75</v>
       </c>
       <c r="I45" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="J45" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>90</v>
+        <v>56</v>
       </c>
       <c r="K45" s="8"/>
     </row>
@@ -3640,13 +3640,13 @@
         <v>51</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>100</v>
+        <v>202</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>153</v>
+        <v>103</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>202</v>
+        <v>152</v>
       </c>
       <c r="E46" s="7" t="s">
         <v>10</v>
@@ -3655,20 +3655,20 @@
         <v>7</v>
       </c>
       <c r="G46" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>84</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>96</v>
       </c>
       <c r="H46" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>64</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>99</v>
       </c>
       <c r="I46" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="J46" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="K46" s="8"/>
     </row>
@@ -3677,13 +3677,13 @@
         <v>52</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>101</v>
+        <v>203</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>154</v>
+        <v>104</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>203</v>
+        <v>153</v>
       </c>
       <c r="E47" s="7" t="s">
         <v>10</v>
@@ -3692,20 +3692,20 @@
         <v>7</v>
       </c>
       <c r="G47" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>75</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>95</v>
       </c>
       <c r="H47" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>72</v>
       </c>
       <c r="I47" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="J47" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="K47" s="8"/>
     </row>
@@ -3714,13 +3714,13 @@
         <v>53</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>102</v>
+        <v>204</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>204</v>
+        <v>154</v>
       </c>
       <c r="E48" s="7" t="s">
         <v>10</v>
@@ -3729,20 +3729,20 @@
         <v>7</v>
       </c>
       <c r="G48" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>13</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>94</v>
       </c>
       <c r="H48" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>62</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>93</v>
       </c>
       <c r="I48" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="J48" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>93</v>
+        <v>45</v>
       </c>
       <c r="K48" s="8"/>
     </row>
@@ -3751,13 +3751,13 @@
         <v>54</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>103</v>
+        <v>205</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>156</v>
+        <v>106</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>205</v>
+        <v>155</v>
       </c>
       <c r="E49" s="7" t="s">
         <v>10</v>
@@ -3766,20 +3766,20 @@
         <v>7</v>
       </c>
       <c r="G49" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>36</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>87</v>
       </c>
       <c r="H49" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>53</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>65</v>
       </c>
       <c r="I49" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="J49" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="K49" s="8"/>
     </row>
@@ -3788,13 +3788,13 @@
         <v>55</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>104</v>
+        <v>206</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>157</v>
+        <v>107</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>206</v>
+        <v>156</v>
       </c>
       <c r="E50" s="7" t="s">
         <v>10</v>
@@ -3803,20 +3803,20 @@
         <v>7</v>
       </c>
       <c r="G50" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>48</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>61</v>
       </c>
       <c r="H50" s="9">
-        <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>74</v>
       </c>
       <c r="I50" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="J50" s="9">
         <f t="shared" ca="1" si="1"/>
-        <v>99</v>
+        <v>32</v>
       </c>
       <c r="K50" s="8"/>
     </row>

</xml_diff>